<commit_message>
Laatste bijwerkingen november 2019
</commit_message>
<xml_diff>
--- a/Les 1A - Unplugged - Robot smeert boterham/Verbruikscijfers.xlsx
+++ b/Les 1A - Unplugged - Robot smeert boterham/Verbruikscijfers.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD25254-983A-420C-B0F0-98DA1C076954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="6225"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>doosjes aangebroken</t>
   </si>
@@ -61,13 +69,37 @@
   </si>
   <si>
     <t>gram gebruikt</t>
+  </si>
+  <si>
+    <t>Berekening voor nieuwe klas</t>
+  </si>
+  <si>
+    <t>g margarine</t>
+  </si>
+  <si>
+    <t>kuipjes van 250 gram</t>
+  </si>
+  <si>
+    <t>g hagelslag</t>
+  </si>
+  <si>
+    <t>doosjes hagelslag van 250 gram</t>
+  </si>
+  <si>
+    <t>leerlingen + begeleiders</t>
+  </si>
+  <si>
+    <t>sneetjes</t>
+  </si>
+  <si>
+    <t>broden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +110,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -104,22 +144,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,9 +207,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -191,9 +241,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,9 +293,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,21 +486,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>46</v>
       </c>
@@ -422,7 +508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>25</v>
       </c>
@@ -430,7 +516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3</f>
         <v>25</v>
@@ -439,12 +525,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75">
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>(273+266)/2</f>
         <v>269.5</v>
@@ -453,7 +539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -461,7 +547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>788</v>
       </c>
@@ -469,7 +555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>A10*A9-A11</f>
         <v>559.5</v>
@@ -478,8 +564,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <f>A12/A4</f>
         <v>22.38</v>
       </c>
@@ -487,64 +573,131 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18.75">
-      <c r="A15" s="1" t="s">
+    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>269</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>7</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>1683</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
-        <f>A17*A16-A18</f>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>A20*A19-A21</f>
         <v>200</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
-        <f>A19/A4</f>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <f>A22/A4</f>
         <v>8</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18.75">
-      <c r="A22" s="1" t="s">
+    <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>25</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B29" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>A23*A35</f>
+        <v>240</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>ROUNDUP(A36/250,0)</f>
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <f>A13*A35</f>
+        <v>671.4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>ROUNDUP(A38/250,0)</f>
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>A35</f>
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f>ROUNDUP(A40/A29,0)</f>
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -554,24 +707,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Beschrijving aangepast naar 3.0
</commit_message>
<xml_diff>
--- a/Les 1A - Unplugged - Robot smeert boterham/Verbruikscijfers.xlsx
+++ b/Les 1A - Unplugged - Robot smeert boterham/Verbruikscijfers.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD25254-983A-420C-B0F0-98DA1C076954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE6E90F-D00E-4015-A68B-BFF1D926A307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22545" yWindow="3000" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>doosjes aangebroken</t>
   </si>
@@ -77,15 +79,9 @@
     <t>g margarine</t>
   </si>
   <si>
-    <t>kuipjes van 250 gram</t>
-  </si>
-  <si>
     <t>g hagelslag</t>
   </si>
   <si>
-    <t>doosjes hagelslag van 250 gram</t>
-  </si>
-  <si>
     <t>leerlingen + begeleiders</t>
   </si>
   <si>
@@ -93,6 +89,12 @@
   </si>
   <si>
     <t>broden</t>
+  </si>
+  <si>
+    <t>g/pak</t>
+  </si>
+  <si>
+    <t>g/kuipje</t>
   </si>
 </sst>
 </file>
@@ -151,7 +153,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -167,7 +169,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -487,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,41 +635,40 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="30" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>390</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>250</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>30</v>
-      </c>
-      <c r="B35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f>A23*A35</f>
-        <v>240</v>
-      </c>
-      <c r="B36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f>ROUNDUP(A36/250,0)</f>
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <f>A13*A35</f>
-        <v>671.4</v>
+      <c r="A38">
+        <v>47</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
@@ -675,29 +676,58 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>ROUNDUP(A38/250,0)</f>
-        <v>3</v>
+        <f>A23*A38</f>
+        <v>376</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>A35</f>
-        <v>30</v>
-      </c>
-      <c r="B40" t="s">
-        <v>21</v>
+        <f>ROUNDUP(A39/A33,0)</f>
+        <v>2</v>
+      </c>
+      <c r="B40" t="str">
+        <f>_xlfn.CONCAT("kuipjes van ",A33," gram")</f>
+        <v>kuipjes van 250 gram</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <f>ROUNDUP(A40/A29,0)</f>
+      <c r="A41" s="3">
+        <f>A13*A38</f>
+        <v>1051.8599999999999</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f>ROUNDUP(A41/A31,0)</f>
+        <v>3</v>
+      </c>
+      <c r="B42" t="str">
+        <f xml:space="preserve"> _xlfn.CONCAT("doosjes hagelslag van ",A31," gram")</f>
+        <v>doosjes hagelslag van 390 gram</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f>A38</f>
+        <v>47</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f>ROUNDUP(A43/A29,0)</f>
         <v>2</v>
       </c>
-      <c r="B41" t="s">
-        <v>22</v>
+      <c r="B44" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>